<commit_message>
add item rows to stock and consumption log forms
</commit_message>
<xml_diff>
--- a/templates/consumption_log.xlsx
+++ b/templates/consumption_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romuald/Documents/Work/medic/app-services-team/stock-monitoring/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B145B35D-3420-5542-B486-DF5545833E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF42C8B3-5021-3A40-B886-48B5E29CD328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23780" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,10 +18,18 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$M$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$M$38</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -30,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="98">
   <si>
     <t>type</t>
   </si>
@@ -125,12 +133,6 @@
     <t>end group</t>
   </si>
   <si>
-    <t>calculate</t>
-  </si>
-  <si>
-    <t>patient_id</t>
-  </si>
-  <si>
     <t>items</t>
   </si>
   <si>
@@ -164,15 +166,9 @@
     <t>return_note</t>
   </si>
   <si>
-    <t>selected(${reported_stock}, ‘quantity_returned_to_hos’)</t>
-  </si>
-  <si>
     <t>receive_note</t>
   </si>
   <si>
-    <t>selected(${reported_stock}, ‘quantity_received_from_hos’)</t>
-  </si>
-  <si>
     <t>items_received</t>
   </si>
   <si>
@@ -251,15 +247,6 @@
     <t>select_stock_report</t>
   </si>
   <si>
-    <t>quantity_received_from_hos</t>
-  </si>
-  <si>
-    <t>quantity_returned_to_hos</t>
-  </si>
-  <si>
-    <t>Quantity Returned to Health Facility</t>
-  </si>
-  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -291,9 +278,6 @@
   </si>
   <si>
     <t>Quantity Received refers to stock received. Can be either issued by health assistant or any other health facility staff</t>
-  </si>
-  <si>
-    <t>/consumption_log/inputs/contact/_id</t>
   </si>
   <si>
     <r>
@@ -345,12 +329,48 @@
   <si>
     <t>columns</t>
   </si>
+  <si>
+    <t>db:person</t>
+  </si>
+  <si>
+    <t>contact_id</t>
+  </si>
+  <si>
+    <t>db-object</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>../inputs/contact/_id</t>
+  </si>
+  <si>
+    <t>quantity_received</t>
+  </si>
+  <si>
+    <t>quantity_returned</t>
+  </si>
+  <si>
+    <t>Quantity Returned</t>
+  </si>
+  <si>
+    <t>selected(${reported_stock}, ‘quantity_returned’)</t>
+  </si>
+  <si>
+    <t>selected(${reported_stock}, ‘quantity_received’)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -444,12 +464,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
@@ -460,7 +474,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,12 +489,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor rgb="FF76A5AF"/>
+        <fgColor rgb="FFFF7F57"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -488,26 +508,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -543,36 +548,25 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1108,30 +1102,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z36"/>
+  <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.1640625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="52.1640625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9" style="20"/>
-    <col min="5" max="5" width="42" style="20" customWidth="1"/>
-    <col min="6" max="6" width="21" style="20" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" style="20" customWidth="1"/>
-    <col min="8" max="8" width="42.1640625" style="20" customWidth="1"/>
-    <col min="9" max="9" width="38.83203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="9" style="20"/>
-    <col min="11" max="11" width="61.33203125" style="20" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" style="20" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" style="20" customWidth="1"/>
-    <col min="14" max="14" width="15" style="20" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="20"/>
+    <col min="1" max="1" width="35.1640625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="52.1640625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="9" style="18"/>
+    <col min="5" max="5" width="42" style="18" customWidth="1"/>
+    <col min="6" max="6" width="21" style="18" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="42.1640625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="38.83203125" style="18" customWidth="1"/>
+    <col min="10" max="10" width="9" style="18"/>
+    <col min="11" max="11" width="61.33203125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="18" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" style="18" customWidth="1"/>
+    <col min="14" max="14" width="15" style="18" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
@@ -1174,19 +1168,19 @@
       <c r="M1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
     </row>
     <row r="2" spans="1:26" ht="22" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -1300,120 +1294,63 @@
       <c r="Y4" s="16"/>
       <c r="Z4" s="16"/>
     </row>
-    <row r="5" spans="1:26" ht="22" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-    </row>
-    <row r="6" spans="1:26" ht="22" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13">
-        <v>0</v>
-      </c>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
-      <c r="W6" s="30"/>
-      <c r="X6" s="30"/>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="30"/>
-    </row>
-    <row r="7" spans="1:26" ht="22" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
+      <c r="B5" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
     </row>
     <row r="8" spans="1:26" ht="22" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -1439,259 +1376,299 @@
       <c r="Z8" s="16"/>
     </row>
     <row r="9" spans="1:26" ht="22" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13">
+        <v>0</v>
+      </c>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+    </row>
+    <row r="10" spans="1:26" ht="22" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
+    </row>
+    <row r="11" spans="1:26" ht="22" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-    </row>
-    <row r="10" spans="1:26" s="22" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+    </row>
+    <row r="12" spans="1:26" ht="22" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+    </row>
+    <row r="15" spans="1:26" s="13" customFormat="1" ht="66" x14ac:dyDescent="0.15">
+      <c r="A15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="C15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-    </row>
-    <row r="11" spans="1:26" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:26" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-    </row>
-    <row r="13" spans="1:26" s="13" customFormat="1" ht="66" x14ac:dyDescent="0.15">
-      <c r="A13" s="12" t="s">
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+    </row>
+    <row r="16" spans="1:26" s="13" customFormat="1" ht="88" x14ac:dyDescent="0.15">
+      <c r="A16" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
+      <c r="A17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
+      <c r="A18" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="13" customFormat="1" ht="66" x14ac:dyDescent="0.15">
+      <c r="A19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="13" customFormat="1" ht="22" x14ac:dyDescent="0.15">
+      <c r="A20" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+    </row>
+    <row r="21" spans="1:13" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="1:13" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.15"/>
+    <row r="23" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
+      <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12" t="s">
+      <c r="B23" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-    </row>
-    <row r="14" spans="1:26" s="13" customFormat="1" ht="88" x14ac:dyDescent="0.15">
-      <c r="A14" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
-      <c r="A15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
-      <c r="A16" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="13" customFormat="1" ht="66" x14ac:dyDescent="0.15">
-      <c r="A17" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="13" customFormat="1" ht="22" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-    </row>
-    <row r="19" spans="1:13" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.15"/>
-    <row r="20" spans="1:13" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.15"/>
-    <row r="21" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
-      <c r="A21" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-    </row>
-    <row r="22" spans="1:13" s="13" customFormat="1" ht="66" x14ac:dyDescent="0.15">
-      <c r="A22" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" s="13" customFormat="1" ht="22" x14ac:dyDescent="0.15">
-      <c r="A23" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -1700,246 +1677,316 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.15"/>
-    <row r="25" spans="1:13" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+    <row r="24" spans="1:13" s="13" customFormat="1" ht="66" x14ac:dyDescent="0.15">
+      <c r="A24" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="13" customFormat="1" ht="22" x14ac:dyDescent="0.15">
+      <c r="A25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+    </row>
+    <row r="26" spans="1:13" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:13" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B27" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+    </row>
+    <row r="28" spans="1:13" s="24" customFormat="1" ht="88" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+    </row>
+    <row r="30" spans="1:13" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
+      <c r="A31" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-    </row>
-    <row r="26" spans="1:13" s="29" customFormat="1" ht="88" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-    </row>
-    <row r="28" spans="1:13" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
-      <c r="A29" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-    </row>
-    <row r="30" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
-      <c r="A30" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" s="13" customFormat="1" ht="43" x14ac:dyDescent="0.15">
-      <c r="A31" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>59</v>
-      </c>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
     </row>
     <row r="32" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
       <c r="A32" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="13" customFormat="1" ht="43" x14ac:dyDescent="0.15">
       <c r="A33" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" s="13" customFormat="1" ht="22" x14ac:dyDescent="0.15">
+        <v>82</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
       <c r="A34" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
       <c r="A35" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:13" s="13" customFormat="1" ht="22" x14ac:dyDescent="0.15">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="13" customFormat="1" ht="44" x14ac:dyDescent="0.15">
+      <c r="A37" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="13" customFormat="1" ht="22" x14ac:dyDescent="0.15">
+      <c r="A38" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
+      <c r="B38" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A11:V12">
+  <autoFilter ref="A1:M38" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A13:V14">
     <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="calculate">
-      <formula>NOT(ISERROR(SEARCH("calculate",A11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("calculate",A13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:V12">
+  <conditionalFormatting sqref="A13:V14">
     <cfRule type="expression" dxfId="10" priority="5">
-      <formula>AND($A11="begin group", NOT($B11 = ""))</formula>
+      <formula>AND($A13="begin group", NOT($B13 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:V12">
+  <conditionalFormatting sqref="A13:V14">
     <cfRule type="expression" dxfId="9" priority="6">
-      <formula>AND($A11="end group", $B11 = "", $C11 = "", $D11 = "", $E11 = "", $F11 = "", $G11 = "", $H11 = "", $I11 = "", $J11 = "", $K11 = "", $L11 = "", $M11 = "")</formula>
+      <formula>AND($A13="end group", $B13 = "", $C13 = "", $D13 = "", $E13 = "", $F13 = "", $G13 = "", $H13 = "", $I13 = "", $J13 = "", $K13 = "", $L13 = "", $M13 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:V12">
+  <conditionalFormatting sqref="A13:V14">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A12">
+  <conditionalFormatting sqref="A13:A14">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:V12">
+  <conditionalFormatting sqref="A13:V14">
     <cfRule type="expression" dxfId="6" priority="9">
-      <formula>AND($A11="begin repeat", NOT($B11 = ""))</formula>
+      <formula>AND($A13="begin repeat", NOT($B13 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:V12">
+  <conditionalFormatting sqref="A13:V14">
     <cfRule type="expression" dxfId="5" priority="10">
-      <formula>AND($A11="end repeat", $B11 = "", $C11 = "", $D11 = "", $E11 = "", $F11 = "", $G11 = "", $H11 = "", $I11 = "", $J11 = "", $K11 = "", $L11 = "", $M11 = "")</formula>
+      <formula>AND($A13="end repeat", $B13 = "", $C13 = "", $D13 = "", $E13 = "", $F13 = "", $G13 = "", $H13 = "", $I13 = "", $J13 = "", $K13 = "", $L13 = "", $M13 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B12">
+  <conditionalFormatting sqref="B13:B14">
     <cfRule type="expression" dxfId="4" priority="11">
-      <formula>AND(AND(NOT($A11 = "end group"), NOT($A11 = "end repeat"), NOT($A11 = "")), $B11 = "")</formula>
+      <formula>AND(AND(NOT($A13 = "end group"), NOT($A13 = "end repeat"), NOT($A13 = "")), $B13 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C12">
+  <conditionalFormatting sqref="C13:C14">
     <cfRule type="expression" dxfId="3" priority="13">
-      <formula>AND(AND(NOT($A11 = "end group"), NOT($A11 = "end repeat"), NOT($A11 = "")), $C11 = "")</formula>
+      <formula>AND(AND(NOT($A13 = "end group"), NOT($A13 = "end repeat"), NOT($A13 = "")), $C13 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11:H12">
+  <conditionalFormatting sqref="H13:H14">
     <cfRule type="expression" dxfId="2" priority="14">
-      <formula>AND(NOT($G11 = ""), $H11 = "")</formula>
+      <formula>AND(NOT($G13 = ""), $H13 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11:I12">
+  <conditionalFormatting sqref="I13:I14">
     <cfRule type="expression" dxfId="1" priority="15">
       <formula>AND(#REF! = "", #REF! = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B12">
+  <conditionalFormatting sqref="B13:B14">
     <cfRule type="expression" dxfId="0" priority="43">
-      <formula>COUNTIF($B$2:$B$250,B11)&gt;1</formula>
+      <formula>COUNTIF($B$2:$B$254,B13)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="D11:D12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D13:D14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1958,7 +2005,7 @@
   <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1971,7 +2018,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1980,7 +2027,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2007,24 +2054,24 @@
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2049,22 +2096,22 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -2089,19 +2136,19 @@
     </row>
     <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>